<commit_message>
Actualización automática 2025-08-19 14:20:09
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +444,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="28" customWidth="1" min="2" max="2"/>
+    <col width="31" customWidth="1" min="2" max="2"/>
     <col width="25" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="26" customWidth="1" min="5" max="5"/>
@@ -563,7 +563,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>VIEJO RIVAS MAYRA ANABELLE</t>
+          <t>COELLO TRONCOSO JOSE GREGORIO</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -616,84 +616,144 @@
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="K3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="L3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="M3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="N3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="O3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="P3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="Q3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
-        </is>
-      </c>
-      <c r="R3" s="3" t="inlineStr">
-        <is>
-          <t>0 de 1</t>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>VIEJO RIVAS MAYRA ANABELLE</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="N4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="O4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="P4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="Q4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
+        </is>
+      </c>
+      <c r="R4" s="3" t="inlineStr">
+        <is>
+          <t>0 de 2</t>
         </is>
       </c>
     </row>
@@ -708,7 +768,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -717,7 +777,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="28" customWidth="1" min="2" max="2"/>
+    <col width="31" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
@@ -770,7 +830,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>VIEJO RIVAS MAYRA ANABELLE</t>
+          <t>COELLO TRONCOSO JOSE GREGORIO</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -790,19 +850,46 @@
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>VIEJO RIVAS MAYRA ANABELLE</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-08-27 15:05:09
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -803,137 +803,197 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="E7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="F7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="G7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="H7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="I7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="J7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="K7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="L7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="M7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="N7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="O7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="P7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="Q7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="R7" s="3" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="O8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="P8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="Q8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
+        </is>
+      </c>
+      <c r="R8" s="3" t="inlineStr">
+        <is>
+          <t>0 de 6</t>
         </is>
       </c>
     </row>
@@ -948,7 +1008,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1118,39 +1178,66 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4" t="n">
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-01 17:05:06
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -683,7 +683,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>COELLO TRONCOSO JOSE GREGORIO</t>
+          <t>BRITO CARDENAS RUTH CECILIA</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -743,7 +743,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>COMERCIAL LUNA PAZMIÑO CIA. LTDA.</t>
+          <t>COELLO TRONCOSO JOSE GREGORIO</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -803,7 +803,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
+          <t>COMERCIAL LUNA PAZMIÑO CIA. LTDA.</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -863,137 +863,197 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="F8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="H8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="I8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="J8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="K8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="L8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="M8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="N8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="O8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="P8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="Q8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
-        </is>
-      </c>
-      <c r="R8" s="3" t="inlineStr">
-        <is>
-          <t>0 de 6</t>
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="O9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="P9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="Q9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
+        </is>
+      </c>
+      <c r="R9" s="3" t="inlineStr">
+        <is>
+          <t>0 de 7</t>
         </is>
       </c>
     </row>
@@ -1008,7 +1068,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1124,7 +1184,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>COELLO TRONCOSO JOSE GREGORIO</t>
+          <t>BRITO CARDENAS RUTH CECILIA</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -1151,7 +1211,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>COMERCIAL LUNA PAZMIÑO CIA. LTDA.</t>
+          <t>COELLO TRONCOSO JOSE GREGORIO</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -1178,7 +1238,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
+          <t>COMERCIAL LUNA PAZMIÑO CIA. LTDA.</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -1205,39 +1265,66 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4" t="n">
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-01 17:10:07
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +444,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="35" customWidth="1" min="2" max="2"/>
+    <col width="36" customWidth="1" min="2" max="2"/>
     <col width="25" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="26" customWidth="1" min="5" max="5"/>
@@ -863,7 +863,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
+          <t>CORPORACION AREVALO-YUMBLA E HIJOS</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -923,137 +923,197 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="D9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="E9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="F9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="G9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="H9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="I9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="J9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="K9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="L9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="M9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="N9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="O9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="P9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="Q9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
-        </is>
-      </c>
-      <c r="R9" s="3" t="inlineStr">
-        <is>
-          <t>0 de 7</t>
+      <c r="C9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="O10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="P10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="Q10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
+        </is>
+      </c>
+      <c r="R10" s="3" t="inlineStr">
+        <is>
+          <t>0 de 8</t>
         </is>
       </c>
     </row>
@@ -1068,7 +1128,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1077,7 +1137,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="35" customWidth="1" min="2" max="2"/>
+    <col width="36" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
@@ -1265,7 +1325,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
+          <t>CORPORACION AREVALO-YUMBLA E HIJOS</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -1292,39 +1352,66 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4" t="n">
+      <c r="C9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-12 10:30:09
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1043,137 +1043,197 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="E11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="F11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="G11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="H11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="I11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="J11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="K11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="L11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="M11" s="3" t="inlineStr">
-        <is>
-          <t>2 de 9</t>
-        </is>
-      </c>
-      <c r="N11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="O11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="P11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="Q11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
-        </is>
-      </c>
-      <c r="R11" s="3" t="inlineStr">
-        <is>
-          <t>0 de 9</t>
+      <c r="C11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>2 de 10</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="O12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="P12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="Q12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
+        </is>
+      </c>
+      <c r="R12" s="3" t="inlineStr">
+        <is>
+          <t>0 de 10</t>
         </is>
       </c>
     </row>
@@ -1188,7 +1248,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1466,39 +1526,66 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" s="4" t="n">
+      <c r="C11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="4" t="n">
         <v>1187.62</v>
       </c>
-      <c r="D11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4" t="n">
+      <c r="D12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4" t="n">
         <v>5415.120000000001</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G12" s="4" t="n">
         <v>1200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-26 12:55:09
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -623,7 +623,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BRAVO MONTENEGRO DANIEL ANDRES</t>
+          <t>BARROS YUNGA DIEGO VINICIO</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -683,7 +683,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BRITO CARDENAS RUTH CECILIA</t>
+          <t>BRAVO MONTENEGRO DANIEL ANDRES</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -743,7 +743,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>COELLO TRONCOSO JOSE GREGORIO</t>
+          <t>BRITO CARDENAS RUTH CECILIA</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -803,7 +803,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>COMERCIAL LUNA PAZMIÑO CIA. LTDA.</t>
+          <t>COELLO TRONCOSO JOSE GREGORIO</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -863,7 +863,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CORPORACION AREVALO-YUMBLA E HIJOS</t>
+          <t>COMERCIAL LUNA PAZMIÑO CIA. LTDA.</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -923,7 +923,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>FABIMP BENIGNO BRAVO S.A.S.</t>
+          <t>CORPORACION AREVALO-YUMBLA E HIJOS</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>43.1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="2" t="n">
         <v>0</v>
@@ -983,7 +983,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
+          <t>FABIMP BENIGNO BRAVO S.A.S.</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1017,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>5372.02</v>
+        <v>43.1</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>0</v>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>122.67</v>
+        <v>5372.02</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -1086,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="2" t="n">
-        <v>13.81</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="2" t="n">
         <v>0</v>
@@ -1103,7 +1103,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MOROCHO BACUILIMA HILDA INES</t>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0</v>
+        <v>122.67</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>0</v>
@@ -1146,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="2" t="n">
-        <v>0</v>
+        <v>13.81</v>
       </c>
       <c r="Q11" s="2" t="n">
         <v>0</v>
@@ -1163,137 +1163,197 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>MOROCHO BACUILIMA HILDA INES</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="C13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="D13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="E13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="F13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="G13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="H13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="I13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="J13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="K13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="L13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="M13" s="3" t="inlineStr">
-        <is>
-          <t>3 de 11</t>
-        </is>
-      </c>
-      <c r="N13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="O13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="P13" s="3" t="inlineStr">
-        <is>
-          <t>1 de 11</t>
-        </is>
-      </c>
-      <c r="Q13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-      <c r="R13" s="3" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
+      <c r="C13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>3 de 12</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="O14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="P14" s="3" t="inlineStr">
+        <is>
+          <t>1 de 12</t>
+        </is>
+      </c>
+      <c r="Q14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
+        </is>
+      </c>
+      <c r="R14" s="3" t="inlineStr">
+        <is>
+          <t>0 de 12</t>
         </is>
       </c>
     </row>
@@ -1308,7 +1368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1397,7 +1457,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BRAVO MONTENEGRO DANIEL ANDRES</t>
+          <t>BARROS YUNGA DIEGO VINICIO</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -1424,7 +1484,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BRITO CARDENAS RUTH CECILIA</t>
+          <t>BRAVO MONTENEGRO DANIEL ANDRES</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -1451,7 +1511,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>COELLO TRONCOSO JOSE GREGORIO</t>
+          <t>BRITO CARDENAS RUTH CECILIA</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -1478,7 +1538,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>COMERCIAL LUNA PAZMIÑO CIA. LTDA.</t>
+          <t>COELLO TRONCOSO JOSE GREGORIO</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -1505,7 +1565,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CORPORACION AREVALO-YUMBLA E HIJOS</t>
+          <t>COMERCIAL LUNA PAZMIÑO CIA. LTDA.</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -1532,11 +1592,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>FABIMP BENIGNO BRAVO S.A.S.</t>
+          <t>CORPORACION AREVALO-YUMBLA E HIJOS</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>1187.62</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>0</v>
@@ -1545,10 +1605,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>43.1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1559,11 +1619,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
+          <t>FABIMP BENIGNO BRAVO S.A.S.</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0</v>
+        <v>1187.62</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>0</v>
@@ -1572,10 +1632,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>5372.02</v>
+        <v>43.1</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="10">
@@ -1586,7 +1646,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+          <t>FRANK FERRETERIA FRANKFERRE CIA.</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1599,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>136.48</v>
+        <v>5372.02</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -1613,7 +1673,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MOROCHO BACUILIMA HILDA INES</t>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1626,7 +1686,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0</v>
+        <v>136.48</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>0</v>
@@ -1640,39 +1700,66 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>MOROCHO BACUILIMA HILDA INES</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="C13" s="4" t="n">
+      <c r="C13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="4" t="n">
         <v>1187.62</v>
       </c>
-      <c r="D13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="4" t="n">
+      <c r="D14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4" t="n">
         <v>5551.6</v>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G14" s="4" t="n">
         <v>1200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-10-14 16:30:09
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +444,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="36" customWidth="1" min="2" max="2"/>
+    <col width="41" customWidth="1" min="2" max="2"/>
     <col width="25" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
     <col width="26" customWidth="1" min="5" max="5"/>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MOROCHO BACUILIMA HILDA INES</t>
+          <t>MIM CONSTRUFERRETERIA E IMPORTADORA SAS</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
+          <t>MOROCHO BACUILIMA HILDA INES</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1283,137 +1283,197 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="D15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="E15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="G15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="H15" s="3" t="inlineStr">
-        <is>
-          <t>3 de 13</t>
-        </is>
-      </c>
-      <c r="I15" s="3" t="inlineStr">
-        <is>
-          <t>1 de 13</t>
-        </is>
-      </c>
-      <c r="J15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="K15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="L15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="M15" s="3" t="inlineStr">
-        <is>
-          <t>2 de 13</t>
-        </is>
-      </c>
-      <c r="N15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="O15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="P15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="Q15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
-        </is>
-      </c>
-      <c r="R15" s="3" t="inlineStr">
-        <is>
-          <t>0 de 13</t>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>3 de 14</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>1 de 14</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>2 de 14</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="O16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="P16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="Q16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
+        </is>
+      </c>
+      <c r="R16" s="3" t="inlineStr">
+        <is>
+          <t>0 de 14</t>
         </is>
       </c>
     </row>
@@ -1428,7 +1488,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1437,7 +1497,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="36" customWidth="1" min="2" max="2"/>
+    <col width="41" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="16" customWidth="1" min="5" max="5"/>
@@ -1760,7 +1820,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MOROCHO BACUILIMA HILDA INES</t>
+          <t>MIM CONSTRUFERRETERIA E IMPORTADORA SAS</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1770,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>102.6</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>0</v>
@@ -1787,7 +1847,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
+          <t>MOROCHO BACUILIMA HILDA INES</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1797,7 +1857,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0</v>
+        <v>102.6</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0</v>
@@ -1814,39 +1874,66 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="4" t="n">
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4" t="n">
         <v>6606.64</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F16" s="4" t="n">
         <v>6512.77</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G16" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-10-15 09:30:09
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
+          <t>MULLO GUACHO ANA LUCIA</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1343,137 +1343,197 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="H16" s="3" t="inlineStr">
-        <is>
-          <t>3 de 14</t>
-        </is>
-      </c>
-      <c r="I16" s="3" t="inlineStr">
-        <is>
-          <t>1 de 14</t>
-        </is>
-      </c>
-      <c r="J16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="K16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="L16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="M16" s="3" t="inlineStr">
-        <is>
-          <t>3 de 14</t>
-        </is>
-      </c>
-      <c r="N16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="O16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="P16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="Q16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
-        </is>
-      </c>
-      <c r="R16" s="3" t="inlineStr">
-        <is>
-          <t>0 de 14</t>
+      <c r="C16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>3 de 15</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>1 de 15</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>3 de 15</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="O17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="P17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="Q17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
+        </is>
+      </c>
+      <c r="R17" s="3" t="inlineStr">
+        <is>
+          <t>0 de 15</t>
         </is>
       </c>
     </row>
@@ -1488,7 +1548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1874,7 +1934,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
+          <t>MULLO GUACHO ANA LUCIA</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1901,39 +1961,66 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4" t="n">
+      <c r="C16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="n">
         <v>6606.64</v>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F17" s="4" t="n">
         <v>7571.12</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G17" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-10-15 17:30:09
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -1017,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>0</v>
+        <v>252.25</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>0</v>
@@ -1362,10 +1362,10 @@
         <v>0</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>0</v>
+        <v>205.2</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>0</v>
+        <v>85.5</v>
       </c>
       <c r="J15" s="2" t="n">
         <v>0</v>
@@ -1483,12 +1483,12 @@
       </c>
       <c r="H17" s="3" t="inlineStr">
         <is>
-          <t>3 de 15</t>
+          <t>4 de 15</t>
         </is>
       </c>
       <c r="I17" s="3" t="inlineStr">
         <is>
-          <t>1 de 15</t>
+          <t>2 de 15</t>
         </is>
       </c>
       <c r="J17" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
       </c>
       <c r="M17" s="3" t="inlineStr">
         <is>
-          <t>3 de 15</t>
+          <t>4 de 15</t>
         </is>
       </c>
       <c r="N17" s="3" t="inlineStr">
@@ -1812,7 +1812,7 @@
         <v>400.46</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0</v>
+        <v>252.25</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>0</v>
@@ -1974,7 +1974,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>0</v>
+        <v>290.7</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>0</v>
@@ -2018,7 +2018,7 @@
         <v>6606.64</v>
       </c>
       <c r="F17" s="4" t="n">
-        <v>7571.12</v>
+        <v>8114.07</v>
       </c>
       <c r="G17" s="4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-11-19 08:30:08
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1103,7 +1103,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+          <t>HUERTA MUÑOZ NANCY ELIZABETH</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>162.19</v>
+        <v>0</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>0</v>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MIM CONSTRUFERRETERIA E IMPORTADORA SAS</t>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>0</v>
+        <v>162.19</v>
       </c>
       <c r="N12" s="2" t="n">
         <v>0</v>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MOROCHO BACUILIMA HILDA INES</t>
+          <t>MIM CONSTRUFERRETERIA E IMPORTADORA SAS</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MULLO GUACHO ANA LUCIA</t>
+          <t>MOROCHO BACUILIMA HILDA INES</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
+          <t>MULLO GUACHO ANA LUCIA</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ROCAFUERTE LOPEZ EVELYN ESTEFANIA</t>
+          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1463,137 +1463,197 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>ROCAFUERTE LOPEZ EVELYN ESTEFANIA</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="D18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="E18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="F18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="G18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="H18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="I18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="J18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="K18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="L18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="M18" s="3" t="inlineStr">
-        <is>
-          <t>2 de 16</t>
-        </is>
-      </c>
-      <c r="N18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="O18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="P18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="Q18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
-        </is>
-      </c>
-      <c r="R18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 16</t>
+      <c r="C18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>2 de 17</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="O19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="P19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="Q19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
+        </is>
+      </c>
+      <c r="R19" s="3" t="inlineStr">
+        <is>
+          <t>0 de 17</t>
         </is>
       </c>
     </row>
@@ -1608,7 +1668,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1913,20 +1973,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+          <t>HUERTA MUÑOZ NANCY ELIZABETH</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>136.48</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>58.48</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>162.19</v>
+        <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>0</v>
@@ -1940,20 +2000,20 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MIM CONSTRUFERRETERIA E IMPORTADORA SAS</t>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0</v>
+        <v>136.48</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>3896.18</v>
+        <v>58.48</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0</v>
+        <v>162.19</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>0</v>
@@ -1967,17 +2027,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MOROCHO BACUILIMA HILDA INES</t>
+          <t>MIM CONSTRUFERRETERIA E IMPORTADORA SAS</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>102.6</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0</v>
+        <v>3896.18</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0</v>
@@ -1994,14 +2054,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MULLO GUACHO ANA LUCIA</t>
+          <t>MOROCHO BACUILIMA HILDA INES</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0</v>
+        <v>102.6</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>0</v>
@@ -2021,7 +2081,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
+          <t>MULLO GUACHO ANA LUCIA</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -2031,7 +2091,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>326.73</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0</v>
@@ -2048,7 +2108,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ROCAFUERTE LOPEZ EVELYN ESTEFANIA</t>
+          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -2058,7 +2118,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>1015.74</v>
+        <v>326.73</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>0</v>
@@ -2075,39 +2135,66 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>ROCAFUERTE LOPEZ EVELYN ESTEFANIA</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>1015.74</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="4" t="n">
+      <c r="C18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4" t="n">
         <v>6606.64</v>
       </c>
-      <c r="E18" s="4" t="n">
+      <c r="E19" s="4" t="n">
         <v>17222.84</v>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F19" s="4" t="n">
         <v>1793.34</v>
       </c>
-      <c r="G18" s="4" t="n">
+      <c r="G19" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-11-27 12:30:09
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -597,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>0</v>
+        <v>797.36</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>0</v>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="M20" s="3" t="inlineStr">
         <is>
-          <t>2 de 18</t>
+          <t>3 de 18</t>
         </is>
       </c>
       <c r="N20" s="3" t="inlineStr">
@@ -1803,7 +1803,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0</v>
+        <v>797.36</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>0</v>
@@ -2279,7 +2279,7 @@
         <v>17222.84</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>2326.47</v>
+        <v>3123.83</v>
       </c>
       <c r="G20" s="4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-12-04 10:30:07
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1583,137 +1583,197 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>SARMIENTO SARMIENTO SANDRA EULALIA</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="C20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="D20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="E20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="F20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="G20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="H20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="I20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="J20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="K20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="L20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="M20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="N20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="O20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="P20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="Q20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
-        </is>
-      </c>
-      <c r="R20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 18</t>
+      <c r="C20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="E21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="G21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="O21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="P21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="Q21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
+        </is>
+      </c>
+      <c r="R21" s="3" t="inlineStr">
+        <is>
+          <t>0 de 19</t>
         </is>
       </c>
     </row>
@@ -1728,7 +1788,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2249,39 +2309,66 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>SARMIENTO SARMIENTO SANDRA EULALIA</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="C20" s="4" t="n">
+      <c r="C20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="4" t="n">
         <v>6606.64</v>
       </c>
-      <c r="D20" s="4" t="n">
+      <c r="D21" s="4" t="n">
         <v>17222.84</v>
       </c>
-      <c r="E20" s="4" t="n">
+      <c r="E21" s="4" t="n">
         <v>3750.24</v>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F21" s="4" t="n">
         <v>-591.61</v>
       </c>
-      <c r="G20" s="4" t="n">
+      <c r="G21" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-12-07 17:54:30
</commit_message>
<xml_diff>
--- a/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
+++ b/data/ILLER LOPEZ ROBERTO FERNANDO.xlsx
@@ -1788,7 +1788,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2282,23 +2282,23 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>PAUTA ASTUDILLO JULIO HERNAN</t>
+          <t>ROCAFUERTE LOPEZ EVELYN ESTEFANIA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>326.73</v>
+        <v>1015.74</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>0</v>
+        <v>1218.02</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0</v>
+        <v>-591.61</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -2309,20 +2309,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ROCAFUERTE LOPEZ EVELYN ESTEFANIA</t>
+          <t>SARMIENTO SARMIENTO SANDRA EULALIA</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>1015.74</v>
+        <v>0</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>1218.02</v>
+        <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>-591.61</v>
+        <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>0</v>
@@ -2336,7 +2336,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SARMIENTO SARMIENTO SANDRA EULALIA</t>
+          <t>VIEJO RIVAS MAYRA ANABELLE</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -2356,47 +2356,20 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>ILLER LOPEZ ROBERTO FERNANDO</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>VIEJO RIVAS MAYRA ANABELLE</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="C22" s="4" t="n">
+      <c r="C21" s="4" t="n">
         <v>6606.64</v>
       </c>
-      <c r="D22" s="4" t="n">
-        <v>17549.57</v>
-      </c>
-      <c r="E22" s="4" t="n">
+      <c r="D21" s="4" t="n">
+        <v>17222.84</v>
+      </c>
+      <c r="E21" s="4" t="n">
         <v>3750.24</v>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F21" s="4" t="n">
         <v>-497.62</v>
       </c>
-      <c r="G22" s="4" t="n">
-        <v>1000</v>
+      <c r="G21" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>